<commit_message>
update 20240628 by xhx
</commit_message>
<xml_diff>
--- a/rules/rules.xlsx
+++ b/rules/rules.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,17 +10,17 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E5695D-6FC1-4D98-9E63-25FB61E4670D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="38">
   <si>
     <t>pID</t>
   </si>
@@ -79,6 +79,66 @@
   <si>
     <t>passive</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pID</t>
+  </si>
+  <si>
+    <t>node0Hint</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>start-end效应部分</t>
+  </si>
+  <si>
+    <t>nodeHint</t>
+  </si>
+  <si>
+    <t>Phase1</t>
+  </si>
+  <si>
+    <t>Phase3</t>
+  </si>
+  <si>
+    <t>第二阶段-位置</t>
+  </si>
+  <si>
+    <t>apType</t>
+  </si>
+  <si>
+    <t>passive</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>protocol</t>
+  </si>
+  <si>
+    <t>test 1</t>
+  </si>
+  <si>
+    <t>test 3</t>
+  </si>
+  <si>
+    <t>SE active2</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>ITI</t>
+  </si>
+  <si>
+    <t>nRepeat</t>
+  </si>
+  <si>
+    <t>cueLag</t>
+  </si>
+  <si>
+    <t>processFcn</t>
   </si>
 </sst>
 </file>
@@ -110,7 +170,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -118,13 +178,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -439,133 +501,452 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="4.109375" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
-    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" customWidth="1"/>
-    <col min="6" max="6" width="5.109375" customWidth="1"/>
-    <col min="7" max="7" width="3.21875" customWidth="1"/>
-    <col min="8" max="8" width="7.88671875" customWidth="1"/>
-    <col min="9" max="9" width="6.77734375" customWidth="1"/>
-    <col min="10" max="10" width="19.6640625" customWidth="1"/>
-    <col min="11" max="11" width="5.109375" customWidth="1"/>
-    <col min="12" max="12" width="8.88671875" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" customWidth="1"/>
-    <col min="14" max="14" width="4" customWidth="1"/>
-    <col min="15" max="15" width="3.77734375" customWidth="1"/>
-    <col min="16" max="16" width="5.21875" customWidth="1"/>
-    <col min="17" max="17" width="3.6640625" customWidth="1"/>
+    <col min="1" max="1" width="3.93359375" customWidth="true"/>
+    <col min="2" max="2" width="16.48828125" customWidth="true"/>
+    <col min="3" max="3" width="13.82421875" customWidth="true"/>
+    <col min="4" max="4" width="7.046875" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="9.37890625" customWidth="true"/>
+    <col min="6" max="6" width="5.15625" customWidth="true"/>
+    <col min="7" max="7" width="3.7109375" customWidth="true"/>
+    <col min="8" max="8" width="7.93359375" customWidth="true"/>
+    <col min="9" max="9" width="6.82421875" customWidth="true"/>
+    <col min="10" max="10" width="10.15625" customWidth="true"/>
+    <col min="11" max="11" width="5.109375" customWidth="true"/>
+    <col min="12" max="12" width="8.88671875" customWidth="true"/>
+    <col min="13" max="13" width="13.33203125" customWidth="true"/>
+    <col min="14" max="14" width="4" customWidth="true"/>
+    <col min="15" max="15" width="3.77734375" customWidth="true"/>
+    <col min="16" max="16" width="5.21875" customWidth="true"/>
+    <col min="17" max="17" width="3.6640625" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="0">
+        <v>4</v>
+      </c>
+      <c r="G2" s="0">
+        <v>4</v>
+      </c>
+      <c r="H2" s="0"/>
+      <c r="I2" s="0"/>
+      <c r="J2" s="0"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="0">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="0">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G3" s="0">
+        <v>4</v>
+      </c>
+      <c r="H3" s="0"/>
+      <c r="I3" s="0"/>
+      <c r="J3" s="0"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="0">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="0">
+        <v>4</v>
+      </c>
+      <c r="G4" s="0">
+        <v>3.5</v>
+      </c>
+      <c r="H4" s="0">
+        <v>40</v>
+      </c>
+      <c r="I4" s="0"/>
+      <c r="J4" s="0"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="0">
+        <v>2</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="0">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G5" s="0">
+        <v>3.5</v>
+      </c>
+      <c r="H5" s="0">
+        <v>40</v>
+      </c>
+      <c r="I5" s="0"/>
+      <c r="J5" s="0"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="0">
+        <v>2</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="0">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="G6" s="0">
+        <v>3.5</v>
+      </c>
+      <c r="H6" s="0">
+        <v>40</v>
+      </c>
+      <c r="I6" s="0"/>
+      <c r="J6" s="0"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="0">
+        <v>2</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="0">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="G7" s="0">
+        <v>3.5</v>
+      </c>
+      <c r="H7" s="0">
+        <v>40</v>
+      </c>
+      <c r="I7" s="0"/>
+      <c r="J7" s="0"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="0">
+        <v>2</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="0">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="G8" s="0">
+        <v>3.5</v>
+      </c>
+      <c r="H8" s="0">
+        <v>40</v>
+      </c>
+      <c r="I8" s="0"/>
+      <c r="J8" s="0"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="0">
+        <v>2</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="0">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="G9" s="0">
+        <v>3.5</v>
+      </c>
+      <c r="H9" s="0">
+        <v>40</v>
+      </c>
+      <c r="I9" s="0"/>
+      <c r="J9" s="0"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="0">
+        <v>2</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="0">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="G10" s="0">
+        <v>3.5</v>
+      </c>
+      <c r="H10" s="0">
+        <v>40</v>
+      </c>
+      <c r="I10" s="0"/>
+      <c r="J10" s="0"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="0">
+        <v>2</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="0">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="G11" s="0">
+        <v>3.5</v>
+      </c>
+      <c r="H11" s="0">
+        <v>40</v>
+      </c>
+      <c r="I11" s="0"/>
+      <c r="J11" s="0"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="0">
+        <v>2</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="0">
+        <v>12</v>
+      </c>
+      <c r="G12" s="0">
+        <v>3.5</v>
+      </c>
+      <c r="H12" s="0">
+        <v>40</v>
+      </c>
+      <c r="I12" s="0"/>
+      <c r="J12" s="0"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="0">
+        <v>2</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="0">
+        <v>13</v>
+      </c>
+      <c r="G13" s="0">
+        <v>3.5</v>
+      </c>
+      <c r="H13" s="0">
+        <v>40</v>
+      </c>
+      <c r="I13" s="0"/>
+      <c r="J13" s="0"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="0">
+        <v>2</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="0">
         <v>14</v>
       </c>
-      <c r="F2">
-        <v>4</v>
-      </c>
-      <c r="G2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="G14" s="0">
+        <v>3.5</v>
+      </c>
+      <c r="H14" s="0">
+        <v>40</v>
+      </c>
+      <c r="I14" s="0"/>
+      <c r="J14" s="0"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="0">
+        <v>2</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="0">
         <v>15</v>
       </c>
-      <c r="F3">
-        <v>4</v>
-      </c>
-      <c r="G3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4">
-        <v>4</v>
-      </c>
-      <c r="G4">
-        <v>4</v>
-      </c>
+      <c r="G15" s="0">
+        <v>3.5</v>
+      </c>
+      <c r="H15" s="0">
+        <v>40</v>
+      </c>
+      <c r="I15" s="0"/>
+      <c r="J15" s="0"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>